<commit_message>
Included all_moments = False in RE class. A few other ongoing development features including normalization of moment deviations by percentage, allowing for constant. allowing for diag plot to use two axises, etc, have not been incorporated in the GMMEst.py
</commit_message>
<xml_diff>
--- a/workingfolder/python/tables/SE_Est.xlsx
+++ b/workingfolder/python/tables/SE_Est.xlsx
@@ -444,7 +444,7 @@
         <v>4</v>
       </c>
       <c r="E2">
-        <v>0.21</v>
+        <v>0.04</v>
       </c>
       <c r="F2">
         <v>0.01</v>
@@ -473,10 +473,10 @@
         <v>5</v>
       </c>
       <c r="E3">
-        <v>0.18</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -488,7 +488,7 @@
         <v>1</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>0.15</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -505,10 +505,10 @@
         <v>5</v>
       </c>
       <c r="E4">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -520,7 +520,7 @@
         <v>1</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>0.15</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -540,10 +540,10 @@
         <v>6</v>
       </c>
       <c r="E5">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -552,13 +552,13 @@
         <v>0.1</v>
       </c>
       <c r="I5">
-        <v>0.02</v>
+        <v>1</v>
       </c>
       <c r="J5">
-        <v>0.03</v>
+        <v>0.15</v>
       </c>
       <c r="K5">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="L5">
         <v>0.1</v>
@@ -578,28 +578,28 @@
         <v>7</v>
       </c>
       <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0.24</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
         <v>0.26</v>
       </c>
-      <c r="F6">
-        <v>0.05</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="I6">
-        <v>0.01</v>
-      </c>
-      <c r="J6">
-        <v>0.03</v>
-      </c>
       <c r="K6">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="L6">
-        <v>1.11</v>
+        <v>2.02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected the following bug: quarterly history is imported as monthly for both DoEstimationwithData and xxSV.
</commit_message>
<xml_diff>
--- a/workingfolder/python/tables/SE_Est.xlsx
+++ b/workingfolder/python/tables/SE_Est.xlsx
@@ -444,10 +444,10 @@
         <v>4</v>
       </c>
       <c r="E2">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="F2">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -473,10 +473,10 @@
         <v>5</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -488,7 +488,7 @@
         <v>1</v>
       </c>
       <c r="J3">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -505,10 +505,10 @@
         <v>5</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -520,7 +520,7 @@
         <v>1</v>
       </c>
       <c r="J4">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -540,25 +540,25 @@
         <v>6</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0.38</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0.88</v>
       </c>
       <c r="H5">
         <v>0.1</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>0.02</v>
       </c>
       <c r="J5">
-        <v>0.15</v>
+        <v>0.03</v>
       </c>
       <c r="K5">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="L5">
         <v>0.1</v>
@@ -578,28 +578,28 @@
         <v>7</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0.38</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0.88</v>
       </c>
       <c r="H6">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="J6">
-        <v>0.26</v>
+        <v>0.03</v>
       </c>
       <c r="K6">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="L6">
-        <v>2.02</v>
+        <v>1.11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>